<commit_message>
added in intitial analysis steps
added formulas and steps for anpp, respiration, and location/season
</commit_message>
<xml_diff>
--- a/results/tr-app-results.xlsx
+++ b/results/tr-app-results.xlsx
@@ -4,12 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27729"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3920" yWindow="380" windowWidth="31380" windowHeight="22640" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="2740" yWindow="1020" windowWidth="34740" windowHeight="22560" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="anpp" sheetId="2" r:id="rId2"/>
     <sheet name="respiration" sheetId="3" r:id="rId3"/>
+    <sheet name="location" sheetId="4" r:id="rId4"/>
+    <sheet name="seasons" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="38">
   <si>
     <t>sample_id</t>
   </si>
@@ -116,13 +118,7 @@
     <t>sample_event_id</t>
   </si>
   <si>
-    <t>o2_change_mg</t>
-  </si>
-  <si>
     <t>time_difference_hr</t>
-  </si>
-  <si>
-    <t>app (mg/hr)</t>
   </si>
   <si>
     <t>anpp_mean (mg/hr)</t>
@@ -135,6 +131,15 @@
   </si>
   <si>
     <t>respiration_std_err</t>
+  </si>
+  <si>
+    <t>same thing as respiration, but select dark bottles instead</t>
+  </si>
+  <si>
+    <t>o2_change_mg/L</t>
+  </si>
+  <si>
+    <t>app (mg/hr*L)</t>
   </si>
 </sst>
 </file>
@@ -183,8 +188,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -197,11 +212,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -479,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P133"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38:D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -532,13 +557,13 @@
         <v>8</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -7550,10 +7575,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7580,10 +7605,65 @@
         <v>26</v>
       </c>
       <c r="F1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G1" t="s">
-        <v>34</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1">
+        <v>42877</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="4">
+        <f>AVERAGE(data!P2:P7)</f>
+        <v>0.72773533924196931</v>
+      </c>
+      <c r="G2">
+        <f>(STDEV(data!P2:P7))/SQRT(COUNT(data!P2:P7))</f>
+        <v>8.8507520949526568E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -7599,9 +7679,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -7610,7 +7692,7 @@
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -7627,10 +7709,15 @@
         <v>26</v>
       </c>
       <c r="F1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="I2" t="s">
         <v>35</v>
-      </c>
-      <c r="G1" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -7641,4 +7728,78 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>